<commit_message>
Diagramme de pert apres modifications
</commit_message>
<xml_diff>
--- a/diagramme-de-pert.xlsx
+++ b/diagramme-de-pert.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kennedy\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kennedy\Desktop\coucou\tpe-SI\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="2364" windowHeight="228"/>
+    <workbookView xWindow="0" yWindow="1200" windowWidth="2364" windowHeight="228"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,15 +24,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>DIAGRAMME DE PERT</t>
   </si>
   <si>
     <t xml:space="preserve">Debut </t>
-  </si>
-  <si>
-    <t>Fin</t>
   </si>
   <si>
     <t>B(3)</t>
@@ -41,63 +38,50 @@
     <t>C(2)</t>
   </si>
   <si>
-    <t>D(2)</t>
-  </si>
-  <si>
-    <t>E(2)</t>
-  </si>
-  <si>
     <t>H(2)</t>
-  </si>
-  <si>
-    <t>I(9)</t>
   </si>
   <si>
     <t>F(3)</t>
   </si>
   <si>
-    <t>G(3)</t>
-  </si>
-  <si>
-    <t>A (6)</t>
-  </si>
-  <si>
-    <t>J(4)</t>
-  </si>
-  <si>
     <t>MARGE</t>
   </si>
   <si>
-    <t>LEGENDES</t>
+    <t>D(3)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>TACHES CRITIQUES</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:  A  ,  B  ,  C    ,  D   ,  E   ,H  ,   I  ,  J</t>
-    </r>
+    <t>E(3)</t>
+  </si>
+  <si>
+    <t>G(2)</t>
+  </si>
+  <si>
+    <t>I(3)</t>
+  </si>
+  <si>
+    <t>J(12)</t>
+  </si>
+  <si>
+    <t>FIN</t>
+  </si>
+  <si>
+    <t>k(5)</t>
+  </si>
+  <si>
+    <t>A (4)</t>
+  </si>
+  <si>
+    <t>LEGENCES DE NOTRE DIAGRAMME DE PERT</t>
+  </si>
+  <si>
+    <t>LE CHEMIN CRITIQUE DE NOTRE DIAGRAMME DE PERT EST : A,B,C,G,H,I,J,K</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,13 +111,6 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -155,7 +132,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -165,13 +142,28 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -347,7 +339,7 @@
                 <a:schemeClr val="bg1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>6</a:t>
+            <a:t>4</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="fr-FR" sz="1100">
@@ -355,7 +347,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>     6</a:t>
+            <a:t>     4</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -416,16 +408,83 @@
                 <a:schemeClr val="bg1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>11  </a:t>
+            <a:t>9   9</a:t>
+          </a:r>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Organigramme : Connecteur 7"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6377940" y="1767840"/>
+          <a:ext cx="754380" cy="784860"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartConnector">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>11</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="fr-FR" sz="1100">
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>  </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
             <a:t>11</a:t>
           </a:r>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -433,25 +492,25 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>30480</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>121920</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>784860</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="Organigramme : Connecteur 7"/>
+        <xdr:cNvPr id="9" name="Organigramme : Connecteur 8"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6377940" y="1767840"/>
+          <a:off x="7955280" y="1775460"/>
           <a:ext cx="754380" cy="784860"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartConnector">
@@ -503,25 +562,25 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>30480</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>784860</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="Organigramme : Connecteur 8"/>
+        <xdr:cNvPr id="10" name="Organigramme : Connecteur 9"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7955280" y="1775460"/>
+          <a:off x="3200400" y="2865120"/>
           <a:ext cx="754380" cy="784860"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartConnector">
@@ -551,77 +610,7 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="fr-FR" sz="1100"/>
-            <a:t>15</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
-            <a:t>  </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="fr-FR" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>15</a:t>
-          </a:r>
-          <a:endParaRPr lang="fr-FR" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>30480</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>121920</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>784860</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="Organigramme : Connecteur 9"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3200400" y="2865120"/>
-          <a:ext cx="754380" cy="784860"/>
-        </a:xfrm>
-        <a:prstGeom prst="flowChartConnector">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="fr-FR" sz="1100"/>
-            <a:t>9     </a:t>
+            <a:t>7     </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="fr-FR" sz="1100">
@@ -629,7 +618,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>9</a:t>
+            <a:t>7</a:t>
           </a:r>
           <a:endParaRPr lang="fr-FR" sz="1100"/>
         </a:p>
@@ -640,14 +629,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>15240</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>769620</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>45720</xdr:colOff>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>175260</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -657,7 +646,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4770120" y="3413760"/>
+          <a:off x="4838700" y="4511040"/>
           <a:ext cx="754380" cy="784860"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartConnector">
@@ -699,7 +688,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>13</a:t>
+            <a:t>10</a:t>
           </a:r>
           <a:endParaRPr lang="fr-FR" sz="1100"/>
         </a:p>
@@ -756,20 +745,12 @@
         <a:p>
           <a:pPr algn="l"/>
           <a:r>
-            <a:rPr lang="fr-FR" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>17</a:t>
-          </a:r>
-          <a:r>
             <a:rPr lang="fr-FR" sz="1100" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="bg1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t> </a:t>
+            <a:t>25 </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="fr-FR" sz="1100">
@@ -777,7 +758,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t> 17</a:t>
+            <a:t> 25</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -866,7 +847,7 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="fr-FR" sz="1100"/>
-            <a:t>26 </a:t>
+            <a:t>30 </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
@@ -878,7 +859,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>26                                  </a:t>
+            <a:t>30                                  </a:t>
           </a:r>
           <a:endParaRPr lang="fr-FR" sz="1100"/>
         </a:p>
@@ -888,100 +869,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>15240</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>769620</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="Organigramme : Connecteur 13"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12694920" y="1760220"/>
-          <a:ext cx="754380" cy="784860"/>
-        </a:xfrm>
-        <a:prstGeom prst="flowChartConnector">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
-            <a:t>30  </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="fr-FR" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>30</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="fr-FR" sz="1100" baseline="0">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="fr-FR" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>    1</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>754380</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -990,7 +887,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6339840" y="3436620"/>
+          <a:off x="6416040" y="4518660"/>
           <a:ext cx="754380" cy="784860"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartConnector">
@@ -1032,26 +929,7 @@
                 <a:schemeClr val="bg1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>15</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="fr-FR" sz="1100" baseline="0">
-            <a:solidFill>
-              <a:schemeClr val="bg1"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="fr-FR" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>2</a:t>
+            <a:t>13</a:t>
           </a:r>
           <a:endParaRPr lang="fr-FR" sz="1100"/>
         </a:p>
@@ -1202,16 +1080,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>68580</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>160020</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>739140</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1220,8 +1098,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4030980" y="3268980"/>
-          <a:ext cx="670560" cy="586740"/>
+          <a:off x="3779520" y="4785360"/>
+          <a:ext cx="975360" cy="121920"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1250,15 +1128,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>53340</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>784860</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>34290</xdr:rowOff>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>11430</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1267,7 +1145,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5600700" y="3863340"/>
+          <a:off x="5631180" y="4937760"/>
           <a:ext cx="731520" cy="11430"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -1484,278 +1362,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>53340</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>784860</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>102870</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="45" name="Connecteur droit avec flèche 44"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11940540" y="2103120"/>
-          <a:ext cx="731520" cy="11430"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>22860</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>220980</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="56" name="Connecteur droit 55"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="7155180" y="3421380"/>
-          <a:ext cx="198120" cy="236220"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>274320</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="59" name="Connecteur droit 58"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="7406640" y="3208020"/>
-          <a:ext cx="144780" cy="175260"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>480060</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>624840</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="60" name="Connecteur droit 59"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="7612380" y="2948940"/>
-          <a:ext cx="144780" cy="190500"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>670560</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="61" name="Connecteur droit 60"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="7802880" y="2712720"/>
-          <a:ext cx="121920" cy="182880"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>30480</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>67940</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>140956</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="66" name="Connecteur droit avec flèche 65"/>
-        <xdr:cNvCxnSpPr>
-          <a:endCxn id="9" idx="3"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="7955280" y="2445380"/>
-          <a:ext cx="110476" cy="221620"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>15240</xdr:colOff>
       <xdr:row>17</xdr:row>
@@ -1845,15 +1451,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>30480</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>784860</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1862,7 +1468,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3200400" y="3291840"/>
+          <a:off x="3208020" y="3246120"/>
           <a:ext cx="754380" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2108,138 +1714,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>754380</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="110" name="Connecteur droit 109"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12679680" y="2186940"/>
-          <a:ext cx="754380" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>22860</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>777240</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="111" name="Connecteur droit 110"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4777740" y="3832860"/>
-          <a:ext cx="754380" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>754380</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="112" name="Connecteur droit 111"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6339840" y="3840480"/>
-          <a:ext cx="754380" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>388620</xdr:colOff>
       <xdr:row>15</xdr:row>
@@ -2375,15 +1849,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>358140</xdr:colOff>
+      <xdr:colOff>320040</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
+      <xdr:rowOff>144780</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
+      <xdr:colOff>323850</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>160020</xdr:rowOff>
+      <xdr:rowOff>175260</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2392,7 +1866,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="5113020" y="1775460"/>
+          <a:off x="5074920" y="1790700"/>
           <a:ext cx="3810" cy="396240"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2594,138 +2068,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>388620</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>392430</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="130" name="Connecteur droit 129"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="13068300" y="1783080"/>
-          <a:ext cx="3810" cy="396240"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>384810</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="131" name="Connecteur droit 130"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="6720840" y="3429000"/>
-          <a:ext cx="3810" cy="396240"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>358140</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="132" name="Connecteur droit 131"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="5113020" y="3429000"/>
-          <a:ext cx="3810" cy="396240"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>769620</xdr:colOff>
       <xdr:row>15</xdr:row>
@@ -3034,60 +2376,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>22860</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="149" name="Connecteur droit 148"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11887200" y="1828800"/>
-          <a:ext cx="815340" cy="7620"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent2"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>624840</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>320040</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>251460</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3096,7 +2394,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="624840" y="5326380"/>
+          <a:off x="6103620" y="6690360"/>
           <a:ext cx="2072640" cy="1950720"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartConnector">
@@ -3147,16 +2445,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>640080</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>693420</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3167,7 +2465,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="640080" y="6316980"/>
+          <a:off x="6118860" y="7680960"/>
           <a:ext cx="914400" cy="914400"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -3193,26 +2491,1029 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>731520</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>754380</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="154" name="Connecteur droit 153"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7071360" y="6690360"/>
+          <a:ext cx="22860" cy="1120140"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>541020</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>220980</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="155" name="Connecteur droit 154"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="6088380" y="7802880"/>
+          <a:ext cx="2057400" cy="15240"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>601980</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>563880</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="62" name="Organigramme : Connecteur 61"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2979420" y="4297680"/>
+          <a:ext cx="754380" cy="784860"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartConnector">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>6</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>    7</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>2</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>640080</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="63" name="Connecteur droit avec flèche 62"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2179320" y="3726180"/>
+          <a:ext cx="838200" cy="723900"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>403860</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>365760</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="67" name="Organigramme : Connecteur 66"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5158740" y="3215640"/>
+          <a:ext cx="754380" cy="784860"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartConnector">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>8 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>  </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>13</a:t>
+          </a:r>
+          <a:endParaRPr lang="fr-FR" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="68" name="Connecteur droit avec flèche 67"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4015740" y="3406140"/>
+          <a:ext cx="1028700" cy="167640"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>106680</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="Connecteur droit 21"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5966460" y="3337560"/>
+          <a:ext cx="480060" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>632460</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="78" name="Connecteur droit 77"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="6492240" y="3070860"/>
+          <a:ext cx="480060" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>693420</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="79" name="Connecteur droit 78"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7033260" y="2796540"/>
+          <a:ext cx="480060" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>655320</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>137160</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="80" name="Connecteur droit 79"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="6995160" y="4175760"/>
+          <a:ext cx="274320" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>198120</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>472440</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="85" name="Connecteur droit 84"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7330440" y="3771900"/>
+          <a:ext cx="274320" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>510540</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>784860</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="86" name="Connecteur droit 85"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7642860" y="3352800"/>
+          <a:ext cx="274320" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>15240</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="87" name="Connecteur droit 86"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7940040" y="2964180"/>
+          <a:ext cx="274320" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>320040</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="31" name="Connecteur droit avec flèche 30"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="8244840" y="2552700"/>
+          <a:ext cx="251460" cy="358140"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>426720</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="91" name="Connecteur droit avec flèche 90"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7559040" y="2514600"/>
+          <a:ext cx="487680" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>769620</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>773430</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="94" name="Connecteur droit 93"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="5524500" y="3200400"/>
+          <a:ext cx="3810" cy="396240"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>422910</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="95" name="Connecteur droit 94"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="5173980" y="4503420"/>
+          <a:ext cx="3810" cy="396240"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>449580</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>453390</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="96" name="Connecteur droit 95"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6789420" y="4518660"/>
+          <a:ext cx="3810" cy="396240"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>175260</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>179070</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="97" name="Connecteur droit 96"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="3345180" y="4290060"/>
+          <a:ext cx="3810" cy="396240"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="98" name="Connecteur droit 97"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2971800" y="4686300"/>
+          <a:ext cx="754380" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>373380</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>335280</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="99" name="Connecteur droit 98"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5128260" y="3604260"/>
+          <a:ext cx="754380" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="154" name="Connecteur droit 153"/>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="101" name="Connecteur droit 100"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1600200" y="5326380"/>
-          <a:ext cx="22860" cy="1120140"/>
+          <a:off x="4831080" y="4930140"/>
+          <a:ext cx="754380" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -3237,26 +3538,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>617220</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>297180</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="155" name="Connecteur droit 154"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="617220" y="6469380"/>
-          <a:ext cx="2057400" cy="15240"/>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>45720</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="102" name="Connecteur droit 101"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6385560" y="4914900"/>
+          <a:ext cx="754380" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -3545,10 +3846,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:R41"/>
+  <dimension ref="A2:R51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:R49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3557,58 +3858,57 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D6" s="2"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="Q9" s="1" t="s">
-        <v>2</v>
+      <c r="O9" s="3" t="s">
+        <v>12</v>
       </c>
+      <c r="Q9" s="1"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="H11" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
-      <c r="P11" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="P11" s="1"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G15" s="1">
         <v>0</v>
@@ -3625,21 +3925,19 @@
       <c r="O15" s="1">
         <v>0</v>
       </c>
-      <c r="Q15" s="1">
-        <v>0</v>
-      </c>
+      <c r="Q15" s="1"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="F19" s="1" t="s">
-        <v>9</v>
+      <c r="F19" s="8" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
@@ -3652,73 +3950,461 @@
       <c r="E21" s="1">
         <v>0</v>
       </c>
-      <c r="H21" s="1" t="s">
-        <v>10</v>
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="D22" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="G23">
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="G24" s="1">
-        <v>4</v>
-      </c>
-      <c r="I24" s="1">
-        <v>4</v>
+      <c r="G24" s="1"/>
+      <c r="I24" s="1"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="F26" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="H27" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J27" s="8"/>
+    </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
-        <v>14</v>
+      <c r="A28" s="9"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="9"/>
+      <c r="O28" s="9"/>
+      <c r="P28" s="9"/>
+      <c r="Q28" s="9"/>
+      <c r="R28" s="9"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="E29" s="10">
+        <v>1</v>
       </c>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
-      <c r="L28" s="3"/>
-      <c r="M28" s="3"/>
-      <c r="N28" s="3"/>
-      <c r="O28" s="3"/>
-      <c r="P28" s="3"/>
-      <c r="Q28" s="3"/>
-      <c r="R28" s="3"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="G30" s="3">
+        <v>1</v>
+      </c>
+      <c r="I30" s="3">
+        <v>2</v>
+      </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="O32" s="1"/>
     </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="G33" s="4" t="s">
+    <row r="33" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H33" s="4"/>
-      <c r="I33" s="4"/>
-      <c r="J33" s="4"/>
-      <c r="K33" s="4"/>
-      <c r="L33" s="4"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="11"/>
+      <c r="J33" s="11"/>
+      <c r="K33" s="11"/>
+      <c r="L33" s="11"/>
+      <c r="M33" s="11"/>
+      <c r="N33" s="11"/>
+      <c r="O33" s="11"/>
+      <c r="P33" s="11"/>
+      <c r="Q33" s="11"/>
+      <c r="R33" s="11"/>
     </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
+      <c r="M34" s="4"/>
+      <c r="N34" s="4"/>
+      <c r="O34" s="4"/>
+      <c r="P34" s="4"/>
+      <c r="Q34" s="4"/>
+      <c r="R34" s="4"/>
     </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B41" s="3" t="s">
-        <v>13</v>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
+      <c r="L35" s="4"/>
+      <c r="M35" s="4"/>
+      <c r="N35" s="4"/>
+      <c r="O35" s="4"/>
+      <c r="P35" s="4"/>
+      <c r="Q35" s="4"/>
+      <c r="R35" s="4"/>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
+      <c r="K36" s="4"/>
+      <c r="L36" s="4"/>
+      <c r="M36" s="4"/>
+      <c r="N36" s="4"/>
+      <c r="O36" s="4"/>
+      <c r="P36" s="4"/>
+      <c r="Q36" s="4"/>
+      <c r="R36" s="4"/>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="4"/>
+      <c r="L37" s="4"/>
+      <c r="M37" s="4"/>
+      <c r="N37" s="4"/>
+      <c r="O37" s="4"/>
+      <c r="P37" s="4"/>
+      <c r="Q37" s="4"/>
+      <c r="R37" s="4"/>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="4"/>
+      <c r="L38" s="4"/>
+      <c r="M38" s="4"/>
+      <c r="N38" s="4"/>
+      <c r="O38" s="4"/>
+      <c r="P38" s="4"/>
+      <c r="Q38" s="4"/>
+      <c r="R38" s="4"/>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
+      <c r="K39" s="4"/>
+      <c r="L39" s="4"/>
+      <c r="M39" s="4"/>
+      <c r="N39" s="4"/>
+      <c r="O39" s="4"/>
+      <c r="P39" s="4"/>
+      <c r="Q39" s="4"/>
+      <c r="R39" s="4"/>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="4"/>
+      <c r="K40" s="4"/>
+      <c r="L40" s="4"/>
+      <c r="M40" s="4"/>
+      <c r="N40" s="4"/>
+      <c r="O40" s="4"/>
+      <c r="P40" s="4"/>
+      <c r="Q40" s="4"/>
+      <c r="R40" s="4"/>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="4"/>
+      <c r="K41" s="4"/>
+      <c r="L41" s="4"/>
+      <c r="M41" s="4"/>
+      <c r="N41" s="4"/>
+      <c r="O41" s="4"/>
+      <c r="P41" s="4"/>
+      <c r="Q41" s="4"/>
+      <c r="R41" s="4"/>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4"/>
+      <c r="J42" s="4"/>
+      <c r="K42" s="4"/>
+      <c r="L42" s="4"/>
+      <c r="M42" s="4"/>
+      <c r="N42" s="4"/>
+      <c r="O42" s="4"/>
+      <c r="P42" s="4"/>
+      <c r="Q42" s="4"/>
+      <c r="R42" s="4"/>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="4"/>
+      <c r="J43" s="4"/>
+      <c r="K43" s="4"/>
+      <c r="L43" s="4"/>
+      <c r="M43" s="4"/>
+      <c r="N43" s="4"/>
+      <c r="O43" s="4"/>
+      <c r="P43" s="4"/>
+      <c r="Q43" s="4"/>
+      <c r="R43" s="4"/>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
+      <c r="H44" s="4"/>
+      <c r="I44" s="4"/>
+      <c r="J44" s="4"/>
+      <c r="K44" s="4"/>
+      <c r="L44" s="4"/>
+      <c r="M44" s="4"/>
+      <c r="N44" s="4"/>
+      <c r="O44" s="4"/>
+      <c r="P44" s="4"/>
+      <c r="Q44" s="4"/>
+      <c r="R44" s="4"/>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="4"/>
+      <c r="J45" s="4"/>
+      <c r="K45" s="4"/>
+      <c r="L45" s="4"/>
+      <c r="M45" s="4"/>
+      <c r="N45" s="4"/>
+      <c r="O45" s="4"/>
+      <c r="P45" s="4"/>
+      <c r="Q45" s="4"/>
+      <c r="R45" s="4"/>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
+      <c r="H46" s="4"/>
+      <c r="I46" s="4"/>
+      <c r="J46" s="4"/>
+      <c r="K46" s="4"/>
+      <c r="L46" s="4"/>
+      <c r="M46" s="4"/>
+      <c r="N46" s="4"/>
+      <c r="O46" s="4"/>
+      <c r="P46" s="4"/>
+      <c r="Q46" s="4"/>
+      <c r="R46" s="4"/>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="4"/>
+      <c r="J47" s="4"/>
+      <c r="K47" s="4"/>
+      <c r="L47" s="4"/>
+      <c r="M47" s="4"/>
+      <c r="N47" s="4"/>
+      <c r="O47" s="4"/>
+      <c r="P47" s="4"/>
+      <c r="Q47" s="4"/>
+      <c r="R47" s="4"/>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A48" s="4"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="4"/>
+      <c r="J48" s="4"/>
+      <c r="K48" s="4"/>
+      <c r="L48" s="4"/>
+      <c r="M48" s="4"/>
+      <c r="N48" s="4"/>
+      <c r="O48" s="4"/>
+      <c r="P48" s="4"/>
+      <c r="Q48" s="4"/>
+      <c r="R48" s="4"/>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="4"/>
+      <c r="J49" s="4"/>
+      <c r="K49" s="4"/>
+      <c r="L49" s="4"/>
+      <c r="M49" s="4"/>
+      <c r="N49" s="4"/>
+      <c r="O49" s="4"/>
+      <c r="P49" s="4"/>
+      <c r="Q49" s="4"/>
+      <c r="R49" s="4"/>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A50" s="7" t="s">
+        <v>16</v>
       </c>
-      <c r="C41" s="3"/>
+      <c r="B50" s="7"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="7"/>
+      <c r="H50" s="7"/>
+      <c r="I50" s="7"/>
+      <c r="J50" s="7"/>
+      <c r="K50" s="7"/>
+      <c r="L50" s="7"/>
+      <c r="M50" s="7"/>
+      <c r="N50" s="7"/>
+      <c r="O50" s="7"/>
+      <c r="P50" s="7"/>
+      <c r="Q50" s="7"/>
+      <c r="R50" s="7"/>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A51" s="7"/>
+      <c r="B51" s="7"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7"/>
+      <c r="G51" s="7"/>
+      <c r="H51" s="7"/>
+      <c r="I51" s="7"/>
+      <c r="J51" s="7"/>
+      <c r="K51" s="7"/>
+      <c r="L51" s="7"/>
+      <c r="M51" s="7"/>
+      <c r="N51" s="7"/>
+      <c r="O51" s="7"/>
+      <c r="P51" s="7"/>
+      <c r="Q51" s="7"/>
+      <c r="R51" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="A34:R49"/>
+    <mergeCell ref="A50:R51"/>
     <mergeCell ref="D2:K3"/>
-    <mergeCell ref="A28:R28"/>
-    <mergeCell ref="G33:L34"/>
+    <mergeCell ref="A33:R33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
modification du diagramme de pert pour pouvoir avoir le chemin critique
</commit_message>
<xml_diff>
--- a/diagramme-de-pert.xlsx
+++ b/diagramme-de-pert.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1200" windowWidth="2364" windowHeight="228"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="2364" windowHeight="228"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -59,13 +59,7 @@
     <t>I(3)</t>
   </si>
   <si>
-    <t>J(12)</t>
-  </si>
-  <si>
     <t>FIN</t>
-  </si>
-  <si>
-    <t>k(5)</t>
   </si>
   <si>
     <t>A (4)</t>
@@ -75,6 +69,12 @@
   </si>
   <si>
     <t>LE CHEMIN CRITIQUE DE NOTRE DIAGRAMME DE PERT EST : A,B,C,G,H,I,J,K</t>
+  </si>
+  <si>
+    <t>J(10)</t>
+  </si>
+  <si>
+    <t>k(4)</t>
   </si>
 </sst>
 </file>
@@ -132,7 +132,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -144,15 +144,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -161,6 +152,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -688,7 +691,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>10</a:t>
+            <a:t>13</a:t>
           </a:r>
           <a:endParaRPr lang="fr-FR" sz="1100"/>
         </a:p>
@@ -750,7 +753,7 @@
                 <a:schemeClr val="bg1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>25 </a:t>
+            <a:t>26 </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="fr-FR" sz="1100">
@@ -758,16 +761,8 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t> 25</a:t>
+            <a:t> 26</a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="fr-FR" sz="1100">
-            <a:solidFill>
-              <a:sysClr val="windowText" lastClr="000000"/>
-            </a:solidFill>
-          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
@@ -929,7 +924,7 @@
                 <a:schemeClr val="bg1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>13</a:t>
+            <a:t>16</a:t>
           </a:r>
           <a:endParaRPr lang="fr-FR" sz="1100"/>
         </a:p>
@@ -1269,15 +1264,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
+      <xdr:colOff>449580</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>15240</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>205740</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1285,9 +1280,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8793480" y="2095500"/>
-          <a:ext cx="731520" cy="11430"/>
+        <a:xfrm flipV="1">
+          <a:off x="9166860" y="2621280"/>
+          <a:ext cx="548640" cy="777240"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2288,16 +2283,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>716280</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>22860</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2306,8 +2301,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8717280" y="1828800"/>
-          <a:ext cx="815340" cy="7620"/>
+          <a:off x="8641080" y="2598420"/>
+          <a:ext cx="114300" cy="403860"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2639,7 +2634,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>    7</a:t>
+            <a:t>    10</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2695,16 +2690,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>441960</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>403860</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>365760</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>160020</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2713,7 +2708,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5158740" y="3215640"/>
+          <a:off x="8366760" y="3055620"/>
           <a:ext cx="754380" cy="784860"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartConnector">
@@ -2743,7 +2738,7 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="fr-FR" sz="1100"/>
-            <a:t>8 </a:t>
+            <a:t>16</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
@@ -2755,7 +2750,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>13</a:t>
+            <a:t>16</a:t>
           </a:r>
           <a:endParaRPr lang="fr-FR" sz="1100" baseline="0">
             <a:solidFill>
@@ -2781,26 +2776,114 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>53340</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="68" name="Connecteur droit avec flèche 67"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4015740" y="3406140"/>
-          <a:ext cx="1028700" cy="167640"/>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>472440</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="80" name="Connecteur droit 79"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7216140" y="4572000"/>
+          <a:ext cx="388620" cy="274320"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>510540</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="85" name="Connecteur droit 84"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7642860" y="4267200"/>
+          <a:ext cx="342900" cy="274320"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>99060</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>487680</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="31" name="Connecteur droit avec flèche 30"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="8023860" y="3931920"/>
+          <a:ext cx="388620" cy="312420"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2828,418 +2911,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>106680</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="22" name="Connecteur droit 21"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="5966460" y="3337560"/>
-          <a:ext cx="480060" cy="228600"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>632460</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="78" name="Connecteur droit 77"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="6492240" y="3070860"/>
-          <a:ext cx="480060" cy="228600"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>693420</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="79" name="Connecteur droit 78"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="7033260" y="2796540"/>
-          <a:ext cx="480060" cy="228600"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>655320</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>137160</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="80" name="Connecteur droit 79"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="6995160" y="4175760"/>
-          <a:ext cx="274320" cy="342900"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>198120</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>472440</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="85" name="Connecteur droit 84"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="7330440" y="3771900"/>
-          <a:ext cx="274320" cy="342900"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>510540</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>784860</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="86" name="Connecteur droit 85"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="7642860" y="3352800"/>
-          <a:ext cx="274320" cy="342900"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>15240</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>289560</xdr:colOff>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="87" name="Connecteur droit 86"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="7940040" y="2964180"/>
-          <a:ext cx="274320" cy="342900"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>320040</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="31" name="Connecteur droit avec flèche 30"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="8244840" y="2552700"/>
-          <a:ext cx="251460" cy="358140"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>426720</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>121920</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="91" name="Connecteur droit avec flèche 90"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="7559040" y="2514600"/>
-          <a:ext cx="487680" cy="266700"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>769620</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>773430</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>121920</xdr:rowOff>
+      <xdr:rowOff>160020</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3248,7 +2929,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="5524500" y="3200400"/>
+          <a:off x="8732520" y="3055620"/>
           <a:ext cx="3810" cy="396240"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -3450,16 +3131,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>373380</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>335280</xdr:colOff>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3468,7 +3149,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5128260" y="3604260"/>
+          <a:off x="8382000" y="3474720"/>
           <a:ext cx="754380" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -3572,6 +3253,320 @@
         </a:fillRef>
         <a:effectRef idx="0">
           <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>632460</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="81" name="Connecteur droit avec flèche 80"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8420100" y="2651760"/>
+          <a:ext cx="137160" cy="441960"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>739140</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>312420</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="84" name="Connecteur droit avec flèche 83"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7871460" y="3413760"/>
+          <a:ext cx="365760" cy="129540"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>739140</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="88" name="Connecteur droit 87"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5494020" y="2301240"/>
+          <a:ext cx="548640" cy="274320"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>541020</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="89" name="Connecteur droit 88"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6088380" y="2621280"/>
+          <a:ext cx="480060" cy="220980"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>365760</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>144780</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="90" name="Connecteur droit 89"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6705600" y="2926080"/>
+          <a:ext cx="571500" cy="236220"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="93" name="Connecteur droit 92"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7360920" y="3215640"/>
+          <a:ext cx="457200" cy="144780"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>297180</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="110" name="Connecteur droit 109"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="9364980" y="2819400"/>
+          <a:ext cx="441960" cy="708660"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="tx1"/>
@@ -3848,8 +3843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:R49"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="R30" sqref="R30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3858,33 +3853,33 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D6" s="2"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="O9" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Q9" s="1"/>
     </row>
@@ -3895,11 +3890,9 @@
       <c r="J11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L11" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="L11" s="1"/>
       <c r="N11" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="P11" s="1"/>
     </row>
@@ -3927,18 +3920,28 @@
       </c>
       <c r="Q15" s="1"/>
     </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="K16" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L16" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="L17" s="4"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="J18" s="5"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="F19" s="8" t="s">
-        <v>10</v>
-      </c>
+      <c r="F19" s="5"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
@@ -3956,10 +3959,8 @@
       <c r="D22" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="G23">
-        <v>5</v>
+      <c r="L22" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
@@ -3975,429 +3976,429 @@
       <c r="H27" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J27" s="8"/>
+      <c r="J27" s="5"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A28" s="9"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="9"/>
-      <c r="J28" s="9"/>
-      <c r="K28" s="9"/>
-      <c r="L28" s="9"/>
-      <c r="M28" s="9"/>
-      <c r="N28" s="9"/>
-      <c r="O28" s="9"/>
-      <c r="P28" s="9"/>
-      <c r="Q28" s="9"/>
-      <c r="R28" s="9"/>
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="6"/>
+      <c r="M28" s="6"/>
+      <c r="N28" s="6"/>
+      <c r="O28" s="6"/>
+      <c r="P28" s="6"/>
+      <c r="Q28" s="6"/>
+      <c r="R28" s="6"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="E29" s="10">
-        <v>1</v>
+      <c r="E29" s="7">
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="G30" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I30" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="O32" s="1"/>
     </row>
     <row r="33" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="11" t="s">
-        <v>15</v>
+      <c r="A33" s="12" t="s">
+        <v>13</v>
       </c>
-      <c r="B33" s="11"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="11"/>
-      <c r="J33" s="11"/>
-      <c r="K33" s="11"/>
-      <c r="L33" s="11"/>
-      <c r="M33" s="11"/>
-      <c r="N33" s="11"/>
-      <c r="O33" s="11"/>
-      <c r="P33" s="11"/>
-      <c r="Q33" s="11"/>
-      <c r="R33" s="11"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="12"/>
+      <c r="K33" s="12"/>
+      <c r="L33" s="12"/>
+      <c r="M33" s="12"/>
+      <c r="N33" s="12"/>
+      <c r="O33" s="12"/>
+      <c r="P33" s="12"/>
+      <c r="Q33" s="12"/>
+      <c r="R33" s="12"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
-      <c r="L34" s="4"/>
-      <c r="M34" s="4"/>
-      <c r="N34" s="4"/>
-      <c r="O34" s="4"/>
-      <c r="P34" s="4"/>
-      <c r="Q34" s="4"/>
-      <c r="R34" s="4"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
+      <c r="L34" s="8"/>
+      <c r="M34" s="8"/>
+      <c r="N34" s="8"/>
+      <c r="O34" s="8"/>
+      <c r="P34" s="8"/>
+      <c r="Q34" s="8"/>
+      <c r="R34" s="8"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A35" s="4"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
-      <c r="L35" s="4"/>
-      <c r="M35" s="4"/>
-      <c r="N35" s="4"/>
-      <c r="O35" s="4"/>
-      <c r="P35" s="4"/>
-      <c r="Q35" s="4"/>
-      <c r="R35" s="4"/>
+      <c r="A35" s="8"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="8"/>
+      <c r="K35" s="8"/>
+      <c r="L35" s="8"/>
+      <c r="M35" s="8"/>
+      <c r="N35" s="8"/>
+      <c r="O35" s="8"/>
+      <c r="P35" s="8"/>
+      <c r="Q35" s="8"/>
+      <c r="R35" s="8"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
-      <c r="L36" s="4"/>
-      <c r="M36" s="4"/>
-      <c r="N36" s="4"/>
-      <c r="O36" s="4"/>
-      <c r="P36" s="4"/>
-      <c r="Q36" s="4"/>
-      <c r="R36" s="4"/>
+      <c r="A36" s="8"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="8"/>
+      <c r="L36" s="8"/>
+      <c r="M36" s="8"/>
+      <c r="N36" s="8"/>
+      <c r="O36" s="8"/>
+      <c r="P36" s="8"/>
+      <c r="Q36" s="8"/>
+      <c r="R36" s="8"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A37" s="4"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
-      <c r="H37" s="4"/>
-      <c r="I37" s="4"/>
-      <c r="J37" s="4"/>
-      <c r="K37" s="4"/>
-      <c r="L37" s="4"/>
-      <c r="M37" s="4"/>
-      <c r="N37" s="4"/>
-      <c r="O37" s="4"/>
-      <c r="P37" s="4"/>
-      <c r="Q37" s="4"/>
-      <c r="R37" s="4"/>
+      <c r="A37" s="8"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="8"/>
+      <c r="L37" s="8"/>
+      <c r="M37" s="8"/>
+      <c r="N37" s="8"/>
+      <c r="O37" s="8"/>
+      <c r="P37" s="8"/>
+      <c r="Q37" s="8"/>
+      <c r="R37" s="8"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A38" s="4"/>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="4"/>
-      <c r="I38" s="4"/>
-      <c r="J38" s="4"/>
-      <c r="K38" s="4"/>
-      <c r="L38" s="4"/>
-      <c r="M38" s="4"/>
-      <c r="N38" s="4"/>
-      <c r="O38" s="4"/>
-      <c r="P38" s="4"/>
-      <c r="Q38" s="4"/>
-      <c r="R38" s="4"/>
+      <c r="A38" s="8"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8"/>
+      <c r="K38" s="8"/>
+      <c r="L38" s="8"/>
+      <c r="M38" s="8"/>
+      <c r="N38" s="8"/>
+      <c r="O38" s="8"/>
+      <c r="P38" s="8"/>
+      <c r="Q38" s="8"/>
+      <c r="R38" s="8"/>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A39" s="4"/>
-      <c r="B39" s="4"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
-      <c r="I39" s="4"/>
-      <c r="J39" s="4"/>
-      <c r="K39" s="4"/>
-      <c r="L39" s="4"/>
-      <c r="M39" s="4"/>
-      <c r="N39" s="4"/>
-      <c r="O39" s="4"/>
-      <c r="P39" s="4"/>
-      <c r="Q39" s="4"/>
-      <c r="R39" s="4"/>
+      <c r="A39" s="8"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
+      <c r="K39" s="8"/>
+      <c r="L39" s="8"/>
+      <c r="M39" s="8"/>
+      <c r="N39" s="8"/>
+      <c r="O39" s="8"/>
+      <c r="P39" s="8"/>
+      <c r="Q39" s="8"/>
+      <c r="R39" s="8"/>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A40" s="4"/>
-      <c r="B40" s="4"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
-      <c r="H40" s="4"/>
-      <c r="I40" s="4"/>
-      <c r="J40" s="4"/>
-      <c r="K40" s="4"/>
-      <c r="L40" s="4"/>
-      <c r="M40" s="4"/>
-      <c r="N40" s="4"/>
-      <c r="O40" s="4"/>
-      <c r="P40" s="4"/>
-      <c r="Q40" s="4"/>
-      <c r="R40" s="4"/>
+      <c r="A40" s="8"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="8"/>
+      <c r="I40" s="8"/>
+      <c r="J40" s="8"/>
+      <c r="K40" s="8"/>
+      <c r="L40" s="8"/>
+      <c r="M40" s="8"/>
+      <c r="N40" s="8"/>
+      <c r="O40" s="8"/>
+      <c r="P40" s="8"/>
+      <c r="Q40" s="8"/>
+      <c r="R40" s="8"/>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A41" s="4"/>
-      <c r="B41" s="4"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="4"/>
-      <c r="H41" s="4"/>
-      <c r="I41" s="4"/>
-      <c r="J41" s="4"/>
-      <c r="K41" s="4"/>
-      <c r="L41" s="4"/>
-      <c r="M41" s="4"/>
-      <c r="N41" s="4"/>
-      <c r="O41" s="4"/>
-      <c r="P41" s="4"/>
-      <c r="Q41" s="4"/>
-      <c r="R41" s="4"/>
+      <c r="A41" s="8"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="8"/>
+      <c r="J41" s="8"/>
+      <c r="K41" s="8"/>
+      <c r="L41" s="8"/>
+      <c r="M41" s="8"/>
+      <c r="N41" s="8"/>
+      <c r="O41" s="8"/>
+      <c r="P41" s="8"/>
+      <c r="Q41" s="8"/>
+      <c r="R41" s="8"/>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A42" s="4"/>
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="4"/>
-      <c r="G42" s="4"/>
-      <c r="H42" s="4"/>
-      <c r="I42" s="4"/>
-      <c r="J42" s="4"/>
-      <c r="K42" s="4"/>
-      <c r="L42" s="4"/>
-      <c r="M42" s="4"/>
-      <c r="N42" s="4"/>
-      <c r="O42" s="4"/>
-      <c r="P42" s="4"/>
-      <c r="Q42" s="4"/>
-      <c r="R42" s="4"/>
+      <c r="A42" s="8"/>
+      <c r="B42" s="8"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8"/>
+      <c r="J42" s="8"/>
+      <c r="K42" s="8"/>
+      <c r="L42" s="8"/>
+      <c r="M42" s="8"/>
+      <c r="N42" s="8"/>
+      <c r="O42" s="8"/>
+      <c r="P42" s="8"/>
+      <c r="Q42" s="8"/>
+      <c r="R42" s="8"/>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A43" s="4"/>
-      <c r="B43" s="4"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="4"/>
-      <c r="F43" s="4"/>
-      <c r="G43" s="4"/>
-      <c r="H43" s="4"/>
-      <c r="I43" s="4"/>
-      <c r="J43" s="4"/>
-      <c r="K43" s="4"/>
-      <c r="L43" s="4"/>
-      <c r="M43" s="4"/>
-      <c r="N43" s="4"/>
-      <c r="O43" s="4"/>
-      <c r="P43" s="4"/>
-      <c r="Q43" s="4"/>
-      <c r="R43" s="4"/>
+      <c r="A43" s="8"/>
+      <c r="B43" s="8"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="8"/>
+      <c r="J43" s="8"/>
+      <c r="K43" s="8"/>
+      <c r="L43" s="8"/>
+      <c r="M43" s="8"/>
+      <c r="N43" s="8"/>
+      <c r="O43" s="8"/>
+      <c r="P43" s="8"/>
+      <c r="Q43" s="8"/>
+      <c r="R43" s="8"/>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A44" s="4"/>
-      <c r="B44" s="4"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="4"/>
-      <c r="F44" s="4"/>
-      <c r="G44" s="4"/>
-      <c r="H44" s="4"/>
-      <c r="I44" s="4"/>
-      <c r="J44" s="4"/>
-      <c r="K44" s="4"/>
-      <c r="L44" s="4"/>
-      <c r="M44" s="4"/>
-      <c r="N44" s="4"/>
-      <c r="O44" s="4"/>
-      <c r="P44" s="4"/>
-      <c r="Q44" s="4"/>
-      <c r="R44" s="4"/>
+      <c r="A44" s="8"/>
+      <c r="B44" s="8"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="8"/>
+      <c r="J44" s="8"/>
+      <c r="K44" s="8"/>
+      <c r="L44" s="8"/>
+      <c r="M44" s="8"/>
+      <c r="N44" s="8"/>
+      <c r="O44" s="8"/>
+      <c r="P44" s="8"/>
+      <c r="Q44" s="8"/>
+      <c r="R44" s="8"/>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A45" s="4"/>
-      <c r="B45" s="4"/>
-      <c r="C45" s="4"/>
-      <c r="D45" s="4"/>
-      <c r="E45" s="4"/>
-      <c r="F45" s="4"/>
-      <c r="G45" s="4"/>
-      <c r="H45" s="4"/>
-      <c r="I45" s="4"/>
-      <c r="J45" s="4"/>
-      <c r="K45" s="4"/>
-      <c r="L45" s="4"/>
-      <c r="M45" s="4"/>
-      <c r="N45" s="4"/>
-      <c r="O45" s="4"/>
-      <c r="P45" s="4"/>
-      <c r="Q45" s="4"/>
-      <c r="R45" s="4"/>
+      <c r="A45" s="8"/>
+      <c r="B45" s="8"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="8"/>
+      <c r="I45" s="8"/>
+      <c r="J45" s="8"/>
+      <c r="K45" s="8"/>
+      <c r="L45" s="8"/>
+      <c r="M45" s="8"/>
+      <c r="N45" s="8"/>
+      <c r="O45" s="8"/>
+      <c r="P45" s="8"/>
+      <c r="Q45" s="8"/>
+      <c r="R45" s="8"/>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A46" s="4"/>
-      <c r="B46" s="4"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4"/>
-      <c r="E46" s="4"/>
-      <c r="F46" s="4"/>
-      <c r="G46" s="4"/>
-      <c r="H46" s="4"/>
-      <c r="I46" s="4"/>
-      <c r="J46" s="4"/>
-      <c r="K46" s="4"/>
-      <c r="L46" s="4"/>
-      <c r="M46" s="4"/>
-      <c r="N46" s="4"/>
-      <c r="O46" s="4"/>
-      <c r="P46" s="4"/>
-      <c r="Q46" s="4"/>
-      <c r="R46" s="4"/>
+      <c r="A46" s="8"/>
+      <c r="B46" s="8"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="8"/>
+      <c r="H46" s="8"/>
+      <c r="I46" s="8"/>
+      <c r="J46" s="8"/>
+      <c r="K46" s="8"/>
+      <c r="L46" s="8"/>
+      <c r="M46" s="8"/>
+      <c r="N46" s="8"/>
+      <c r="O46" s="8"/>
+      <c r="P46" s="8"/>
+      <c r="Q46" s="8"/>
+      <c r="R46" s="8"/>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A47" s="4"/>
-      <c r="B47" s="4"/>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
-      <c r="E47" s="4"/>
-      <c r="F47" s="4"/>
-      <c r="G47" s="4"/>
-      <c r="H47" s="4"/>
-      <c r="I47" s="4"/>
-      <c r="J47" s="4"/>
-      <c r="K47" s="4"/>
-      <c r="L47" s="4"/>
-      <c r="M47" s="4"/>
-      <c r="N47" s="4"/>
-      <c r="O47" s="4"/>
-      <c r="P47" s="4"/>
-      <c r="Q47" s="4"/>
-      <c r="R47" s="4"/>
+      <c r="A47" s="8"/>
+      <c r="B47" s="8"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="8"/>
+      <c r="H47" s="8"/>
+      <c r="I47" s="8"/>
+      <c r="J47" s="8"/>
+      <c r="K47" s="8"/>
+      <c r="L47" s="8"/>
+      <c r="M47" s="8"/>
+      <c r="N47" s="8"/>
+      <c r="O47" s="8"/>
+      <c r="P47" s="8"/>
+      <c r="Q47" s="8"/>
+      <c r="R47" s="8"/>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A48" s="4"/>
-      <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="4"/>
-      <c r="G48" s="4"/>
-      <c r="H48" s="4"/>
-      <c r="I48" s="4"/>
-      <c r="J48" s="4"/>
-      <c r="K48" s="4"/>
-      <c r="L48" s="4"/>
-      <c r="M48" s="4"/>
-      <c r="N48" s="4"/>
-      <c r="O48" s="4"/>
-      <c r="P48" s="4"/>
-      <c r="Q48" s="4"/>
-      <c r="R48" s="4"/>
+      <c r="A48" s="8"/>
+      <c r="B48" s="8"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="8"/>
+      <c r="E48" s="8"/>
+      <c r="F48" s="8"/>
+      <c r="G48" s="8"/>
+      <c r="H48" s="8"/>
+      <c r="I48" s="8"/>
+      <c r="J48" s="8"/>
+      <c r="K48" s="8"/>
+      <c r="L48" s="8"/>
+      <c r="M48" s="8"/>
+      <c r="N48" s="8"/>
+      <c r="O48" s="8"/>
+      <c r="P48" s="8"/>
+      <c r="Q48" s="8"/>
+      <c r="R48" s="8"/>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A49" s="4"/>
-      <c r="B49" s="4"/>
-      <c r="C49" s="4"/>
-      <c r="D49" s="4"/>
-      <c r="E49" s="4"/>
-      <c r="F49" s="4"/>
-      <c r="G49" s="4"/>
-      <c r="H49" s="4"/>
-      <c r="I49" s="4"/>
-      <c r="J49" s="4"/>
-      <c r="K49" s="4"/>
-      <c r="L49" s="4"/>
-      <c r="M49" s="4"/>
-      <c r="N49" s="4"/>
-      <c r="O49" s="4"/>
-      <c r="P49" s="4"/>
-      <c r="Q49" s="4"/>
-      <c r="R49" s="4"/>
+      <c r="A49" s="8"/>
+      <c r="B49" s="8"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="8"/>
+      <c r="F49" s="8"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="8"/>
+      <c r="I49" s="8"/>
+      <c r="J49" s="8"/>
+      <c r="K49" s="8"/>
+      <c r="L49" s="8"/>
+      <c r="M49" s="8"/>
+      <c r="N49" s="8"/>
+      <c r="O49" s="8"/>
+      <c r="P49" s="8"/>
+      <c r="Q49" s="8"/>
+      <c r="R49" s="8"/>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A50" s="7" t="s">
-        <v>16</v>
+      <c r="A50" s="9" t="s">
+        <v>14</v>
       </c>
-      <c r="B50" s="7"/>
-      <c r="C50" s="7"/>
-      <c r="D50" s="7"/>
-      <c r="E50" s="7"/>
-      <c r="F50" s="7"/>
-      <c r="G50" s="7"/>
-      <c r="H50" s="7"/>
-      <c r="I50" s="7"/>
-      <c r="J50" s="7"/>
-      <c r="K50" s="7"/>
-      <c r="L50" s="7"/>
-      <c r="M50" s="7"/>
-      <c r="N50" s="7"/>
-      <c r="O50" s="7"/>
-      <c r="P50" s="7"/>
-      <c r="Q50" s="7"/>
-      <c r="R50" s="7"/>
+      <c r="B50" s="9"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
+      <c r="G50" s="9"/>
+      <c r="H50" s="9"/>
+      <c r="I50" s="9"/>
+      <c r="J50" s="9"/>
+      <c r="K50" s="9"/>
+      <c r="L50" s="9"/>
+      <c r="M50" s="9"/>
+      <c r="N50" s="9"/>
+      <c r="O50" s="9"/>
+      <c r="P50" s="9"/>
+      <c r="Q50" s="9"/>
+      <c r="R50" s="9"/>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A51" s="7"/>
-      <c r="B51" s="7"/>
-      <c r="C51" s="7"/>
-      <c r="D51" s="7"/>
-      <c r="E51" s="7"/>
-      <c r="F51" s="7"/>
-      <c r="G51" s="7"/>
-      <c r="H51" s="7"/>
-      <c r="I51" s="7"/>
-      <c r="J51" s="7"/>
-      <c r="K51" s="7"/>
-      <c r="L51" s="7"/>
-      <c r="M51" s="7"/>
-      <c r="N51" s="7"/>
-      <c r="O51" s="7"/>
-      <c r="P51" s="7"/>
-      <c r="Q51" s="7"/>
-      <c r="R51" s="7"/>
+      <c r="A51" s="9"/>
+      <c r="B51" s="9"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="9"/>
+      <c r="H51" s="9"/>
+      <c r="I51" s="9"/>
+      <c r="J51" s="9"/>
+      <c r="K51" s="9"/>
+      <c r="L51" s="9"/>
+      <c r="M51" s="9"/>
+      <c r="N51" s="9"/>
+      <c r="O51" s="9"/>
+      <c r="P51" s="9"/>
+      <c r="Q51" s="9"/>
+      <c r="R51" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>